<commit_message>
[THA Sistemi] Veri Güncelleme
</commit_message>
<xml_diff>
--- a/Personel.xlsx
+++ b/Personel.xlsx
@@ -7,15 +7,15 @@
     <sheet name="ANAMUR" sheetId="2" r:id="rId2"/>
     <sheet name="AYDINCIK" sheetId="3" r:id="rId3"/>
     <sheet name="BOZYAZI" sheetId="4" r:id="rId4"/>
-    <sheet name="ERDEMLİ" sheetId="5" r:id="rId5"/>
-    <sheet name="GÜLNAR" sheetId="6" r:id="rId6"/>
-    <sheet name="MEZİTLİ" sheetId="7" r:id="rId7"/>
-    <sheet name="MUT" sheetId="8" r:id="rId8"/>
-    <sheet name="SİLİFKE" sheetId="9" r:id="rId9"/>
-    <sheet name="TARSUS" sheetId="10" r:id="rId10"/>
-    <sheet name="TOROSLAR" sheetId="11" r:id="rId11"/>
-    <sheet name="YENİŞEHİR" sheetId="12" r:id="rId12"/>
-    <sheet name="ÇAMLIYAYLA" sheetId="13" r:id="rId13"/>
+    <sheet name="ÇAMLIYAYLA" sheetId="5" r:id="rId5"/>
+    <sheet name="ERDEMLİ" sheetId="6" r:id="rId6"/>
+    <sheet name="GÜLNAR" sheetId="7" r:id="rId7"/>
+    <sheet name="MEZİTLİ" sheetId="8" r:id="rId8"/>
+    <sheet name="MUT" sheetId="9" r:id="rId9"/>
+    <sheet name="SİLİFKE" sheetId="10" r:id="rId10"/>
+    <sheet name="TARSUS" sheetId="11" r:id="rId11"/>
+    <sheet name="TOROSLAR" sheetId="12" r:id="rId12"/>
+    <sheet name="YENİŞEHİR" sheetId="13" r:id="rId13"/>
   </sheets>
 </workbook>
 </file>
@@ -713,6 +713,838 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E94"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Mahalle Adı</v>
+      </c>
+      <c r="B1" t="str">
+        <v>GÖREVLİ PERSONEL</v>
+      </c>
+      <c r="C1" t="str">
+        <v>MEGSİS ONAY TARİHİ</v>
+      </c>
+      <c r="D1" t="str">
+        <v>NETİGMA ONAY TARİHİ</v>
+      </c>
+      <c r="E1" t="str">
+        <v>MÜDÜR ONAY</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Akdere</v>
+      </c>
+      <c r="B2" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Akdere/atatürk</v>
+      </c>
+      <c r="B3" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Akdere/cumhuriyet</v>
+      </c>
+      <c r="B4" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Altınkum</v>
+      </c>
+      <c r="B5" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Arkarası</v>
+      </c>
+      <c r="B6" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Atik</v>
+      </c>
+      <c r="B7" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Ayaş türkmenli</v>
+      </c>
+      <c r="B8" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Bahçe</v>
+      </c>
+      <c r="B9" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Bahçederesi</v>
+      </c>
+      <c r="B10" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Balandız</v>
+      </c>
+      <c r="B11" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Bayındır</v>
+      </c>
+      <c r="B12" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Bolacalıkoyuncu</v>
+      </c>
+      <c r="B13" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Boynuinceli</v>
+      </c>
+      <c r="B14" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Bucaklı</v>
+      </c>
+      <c r="B15" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Burunucu</v>
+      </c>
+      <c r="B16" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Bükdeğirmeni</v>
+      </c>
+      <c r="B17" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Cambazlı</v>
+      </c>
+      <c r="B18" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Camikebir</v>
+      </c>
+      <c r="B19" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Cılbayır</v>
+      </c>
+      <c r="B20" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Çadırlı</v>
+      </c>
+      <c r="B21" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Çaltıbozkır</v>
+      </c>
+      <c r="B22" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Çamlıbel</v>
+      </c>
+      <c r="B23" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Çatak</v>
+      </c>
+      <c r="B24" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Çeltikçi</v>
+      </c>
+      <c r="B25" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Demircili</v>
+      </c>
+      <c r="B26" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+      <c r="C26" t="str">
+        <v>2025-09-30</v>
+      </c>
+      <c r="D26" t="str">
+        <v>2025-10-02</v>
+      </c>
+      <c r="E26" t="str">
+        <v>2025-10-03</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Ekşiler</v>
+      </c>
+      <c r="B27" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Esenbel</v>
+      </c>
+      <c r="B28" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Evkafçiftliği</v>
+      </c>
+      <c r="B29" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Gazi</v>
+      </c>
+      <c r="B30" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Gedikpınarı</v>
+      </c>
+      <c r="B31" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Gökbelen</v>
+      </c>
+      <c r="B32" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Gülümpaşalı</v>
+      </c>
+      <c r="B33" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Gümüşlü</v>
+      </c>
+      <c r="B34" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>Gündüzler</v>
+      </c>
+      <c r="B35" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>Hacıishaklı</v>
+      </c>
+      <c r="B36" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Hasanaliler</v>
+      </c>
+      <c r="B37" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Hırmanlı</v>
+      </c>
+      <c r="B38" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Hüseyinler</v>
+      </c>
+      <c r="B39" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Işıklı</v>
+      </c>
+      <c r="B40" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>İmambekirli</v>
+      </c>
+      <c r="B41" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>İmamlı</v>
+      </c>
+      <c r="B42" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+      <c r="C42" t="str">
+        <v>2025-10-01</v>
+      </c>
+      <c r="D42" t="str">
+        <v>2025-10-02</v>
+      </c>
+      <c r="E42" t="str">
+        <v>2025-10-03</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>İmamuşağı</v>
+      </c>
+      <c r="B43" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Kabasakallı</v>
+      </c>
+      <c r="B44" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Kapızlı</v>
+      </c>
+      <c r="B45" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>Karadedeli</v>
+      </c>
+      <c r="B46" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Karahacılı</v>
+      </c>
+      <c r="B47" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>Karakaya</v>
+      </c>
+      <c r="B48" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>Kargıcak</v>
+      </c>
+      <c r="B49" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Kavak</v>
+      </c>
+      <c r="B50" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>Keben</v>
+      </c>
+      <c r="B51" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>Kepez</v>
+      </c>
+      <c r="B52" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>Keşlitürkmenli</v>
+      </c>
+      <c r="B53" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+      <c r="C53" t="str">
+        <v>2025-10-01</v>
+      </c>
+      <c r="D53" t="str">
+        <v>2025-10-02</v>
+      </c>
+      <c r="E53" t="str">
+        <v>2025-10-02</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>Kıca</v>
+      </c>
+      <c r="B54" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>Kızılgeçit</v>
+      </c>
+      <c r="B55" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Kızılisalı</v>
+      </c>
+      <c r="B56" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+      <c r="C56" t="str">
+        <v>2025-10-02</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>Kocaoluk</v>
+      </c>
+      <c r="B57" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>Kocapınar</v>
+      </c>
+      <c r="B58" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>Kurtuluş</v>
+      </c>
+      <c r="B59" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>Mara</v>
+      </c>
+      <c r="B60" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>Mukaddem</v>
+      </c>
+      <c r="B61" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>Mukaddem (a1)</v>
+      </c>
+      <c r="B62" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>Mukaddem(afet)</v>
+      </c>
+      <c r="B63" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>Nasrullah</v>
+      </c>
+      <c r="B64" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>Nuru</v>
+      </c>
+      <c r="B65" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>Olukbaşı</v>
+      </c>
+      <c r="B66" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>Ortaören</v>
+      </c>
+      <c r="B67" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>Ovacık</v>
+      </c>
+      <c r="B68" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+      <c r="C68" t="str">
+        <v>2025-10-02</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>Ören</v>
+      </c>
+      <c r="B69" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>Özboyuninceli</v>
+      </c>
+      <c r="B70" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>Öztürkmenli</v>
+      </c>
+      <c r="B71" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+      <c r="C71" t="str">
+        <v>2025-10-01</v>
+      </c>
+      <c r="D71" t="str">
+        <v>2025-10-02</v>
+      </c>
+      <c r="E71" t="str">
+        <v>2025-10-02</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>Pazarkaşı</v>
+      </c>
+      <c r="B72" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Pelitpınarı</v>
+      </c>
+      <c r="B73" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Sabak</v>
+      </c>
+      <c r="B74" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>Saray</v>
+      </c>
+      <c r="B75" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>Sarıaydın</v>
+      </c>
+      <c r="B76" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>Sarıcalar</v>
+      </c>
+      <c r="B77" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>Say</v>
+      </c>
+      <c r="B78" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>Sayağzı</v>
+      </c>
+      <c r="B79" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>Senir</v>
+      </c>
+      <c r="B80" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>Seydili</v>
+      </c>
+      <c r="B81" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>Seyranlık</v>
+      </c>
+      <c r="B82" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>Sökün</v>
+      </c>
+      <c r="B83" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>Sömek</v>
+      </c>
+      <c r="B84" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>Susanoğlu</v>
+      </c>
+      <c r="B85" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>Şahmurlu</v>
+      </c>
+      <c r="B86" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>Taşucu</v>
+      </c>
+      <c r="B87" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>Tosmurlu</v>
+      </c>
+      <c r="B88" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>Türkmenuşağı</v>
+      </c>
+      <c r="B89" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+      <c r="C89" t="str">
+        <v>2025-10-01</v>
+      </c>
+      <c r="D89" t="str">
+        <v>2025-10-02</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>Ulugöz</v>
+      </c>
+      <c r="B90" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>Uzuncaburç</v>
+      </c>
+      <c r="B91" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>Yeğenli</v>
+      </c>
+      <c r="B92" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>Yenibahçe</v>
+      </c>
+      <c r="B93" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+      <c r="C93" t="str">
+        <v>2025-10-01</v>
+      </c>
+      <c r="D93" t="str">
+        <v>2025-10-02</v>
+      </c>
+      <c r="E93" t="str">
+        <v>2025-10-02</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>Yenisu</v>
+      </c>
+      <c r="B94" t="str">
+        <v>BURAK AKBAŞ</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E94"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E174"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -766,6 +1598,9 @@
       <c r="B5" t="str">
         <v>M. FURKAN KAPLAN</v>
       </c>
+      <c r="C5" t="str">
+        <v>2025-10-03</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -914,7 +1749,7 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Böğrüeğri</v>
+        <v>Bolatlı</v>
       </c>
       <c r="B23" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -922,7 +1757,7 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>Bolatlı</v>
+        <v>Boztepe</v>
       </c>
       <c r="B24" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -930,7 +1765,7 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>Boztepe</v>
+        <v>Böğrüeğri</v>
       </c>
       <c r="B25" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -946,7 +1781,7 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Çağbaşı</v>
+        <v>Camiatik</v>
       </c>
       <c r="B27" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -954,7 +1789,7 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>Çakırlı</v>
+        <v>Camicedit</v>
       </c>
       <c r="B28" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -962,7 +1797,7 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>Çamalan</v>
+        <v>Camilimanda</v>
       </c>
       <c r="B29" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -970,7 +1805,7 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>Camiatik</v>
+        <v>Caminur</v>
       </c>
       <c r="B30" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -978,7 +1813,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Camicedit</v>
+        <v>Cırbıklar</v>
       </c>
       <c r="B31" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -986,7 +1821,7 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Camilimanda</v>
+        <v>Cinköy</v>
       </c>
       <c r="B32" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -994,7 +1829,7 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>Caminur</v>
+        <v>Cumhuriyet</v>
       </c>
       <c r="B33" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -1002,7 +1837,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>Çamtepe</v>
+        <v>Çağbaşı</v>
       </c>
       <c r="B34" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -1010,7 +1845,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>Çataklı</v>
+        <v>Çakırlı</v>
       </c>
       <c r="B35" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -1018,7 +1853,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>Çatalca</v>
+        <v>Çamalan</v>
       </c>
       <c r="B36" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -1026,7 +1861,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>Çatalkeli</v>
+        <v>Çamtepe</v>
       </c>
       <c r="B37" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -1034,7 +1869,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>Çavdarlı</v>
+        <v>Çataklı</v>
       </c>
       <c r="B38" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -1042,7 +1877,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>Çavuşlu</v>
+        <v>Çatalca</v>
       </c>
       <c r="B39" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -1050,7 +1885,7 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>Çevreli</v>
+        <v>Çatalkeli</v>
       </c>
       <c r="B40" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -1058,7 +1893,7 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>Çiftlik</v>
+        <v>Çavdarlı</v>
       </c>
       <c r="B41" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -1066,7 +1901,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>Cinköy</v>
+        <v>Çavuşlu</v>
       </c>
       <c r="B42" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -1074,7 +1909,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>Cırbıklar</v>
+        <v>Çevreli</v>
       </c>
       <c r="B43" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -1082,7 +1917,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>Çiriştepe</v>
+        <v>Çiftlik</v>
       </c>
       <c r="B44" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -1090,7 +1925,7 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>Çokak</v>
+        <v>Çiriştepe</v>
       </c>
       <c r="B45" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -1098,7 +1933,7 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>Çöplü</v>
+        <v>Çokak</v>
       </c>
       <c r="B46" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -1106,7 +1941,7 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>Çukurbağ</v>
+        <v>Çöplü</v>
       </c>
       <c r="B47" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -1114,7 +1949,7 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>Cumhuriyet</v>
+        <v>Çukurbağ</v>
       </c>
       <c r="B48" t="str">
         <v>M. FURKAN KAPLAN</v>
@@ -1570,7 +2405,7 @@
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>Kösebalcı</v>
+        <v>Kozoluk</v>
       </c>
       <c r="B105" t="str">
         <v>RÜYA USLU</v>
@@ -1578,7 +2413,7 @@
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>Köselerli</v>
+        <v>Kösebalcı</v>
       </c>
       <c r="B106" t="str">
         <v>RÜYA USLU</v>
@@ -1586,7 +2421,7 @@
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>Kozoluk</v>
+        <v>Köselerli</v>
       </c>
       <c r="B107" t="str">
         <v>RÜYA USLU</v>
@@ -1594,7 +2429,7 @@
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>Küçükminare</v>
+        <v>Kulak</v>
       </c>
       <c r="B108" t="str">
         <v>RÜYA USLU</v>
@@ -1602,7 +2437,7 @@
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>Kulak</v>
+        <v>Kumdere</v>
       </c>
       <c r="B109" t="str">
         <v>RÜYA USLU</v>
@@ -1610,7 +2445,7 @@
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>Kumdere</v>
+        <v>Kurbanlı</v>
       </c>
       <c r="B110" t="str">
         <v>RÜYA USLU</v>
@@ -1618,7 +2453,7 @@
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>Kurbanlı</v>
+        <v>Kurtçukuru</v>
       </c>
       <c r="B111" t="str">
         <v>RÜYA USLU</v>
@@ -1626,7 +2461,7 @@
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>Kurtçukuru</v>
+        <v>Kuşçular</v>
       </c>
       <c r="B112" t="str">
         <v>RÜYA USLU</v>
@@ -1634,7 +2469,7 @@
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>Kürtmusa</v>
+        <v>Küçükminare</v>
       </c>
       <c r="B113" t="str">
         <v>RÜYA USLU</v>
@@ -1642,7 +2477,7 @@
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>Kuşçular</v>
+        <v>Kürtmusa</v>
       </c>
       <c r="B114" t="str">
         <v>RÜYA USLU</v>
@@ -1690,7 +2525,7 @@
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>Müftü</v>
+        <v>Muratlı</v>
       </c>
       <c r="B120" t="str">
         <v>RÜYA USLU</v>
@@ -1698,7 +2533,7 @@
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>Muratlı</v>
+        <v>Mustafa kemal paşa</v>
       </c>
       <c r="B121" t="str">
         <v>RÜYA USLU</v>
@@ -1706,7 +2541,7 @@
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>Mustafa kemal paşa</v>
+        <v>Müftü</v>
       </c>
       <c r="B122" t="str">
         <v>RÜYA USLU</v>
@@ -1762,7 +2597,7 @@
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>Şahin</v>
+        <v>Sakızlı</v>
       </c>
       <c r="B129" t="str">
         <v>RÜYA USLU</v>
@@ -1770,7 +2605,7 @@
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>Sakızlı</v>
+        <v>Sandal</v>
       </c>
       <c r="B130" t="str">
         <v>RÜYA USLU</v>
@@ -1778,7 +2613,7 @@
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>Sandal</v>
+        <v>Sanlıca</v>
       </c>
       <c r="B131" t="str">
         <v>RÜYA USLU</v>
@@ -1786,7 +2621,7 @@
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>Sanlıca</v>
+        <v>Sarıveli</v>
       </c>
       <c r="B132" t="str">
         <v>RÜYA USLU</v>
@@ -1794,7 +2629,7 @@
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>Sarıveli</v>
+        <v>Sayköy</v>
       </c>
       <c r="B133" t="str">
         <v>RÜYA USLU</v>
@@ -1802,7 +2637,7 @@
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>Sayköy</v>
+        <v>Sıraköy</v>
       </c>
       <c r="B134" t="str">
         <v>RÜYA USLU</v>
@@ -1810,7 +2645,7 @@
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>Şehitisak</v>
+        <v>Simithacılı</v>
       </c>
       <c r="B135" t="str">
         <v>RÜYA USLU</v>
@@ -1818,7 +2653,7 @@
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>Şehitkerim</v>
+        <v>Sofular</v>
       </c>
       <c r="B136" t="str">
         <v>RÜYA USLU</v>
@@ -1826,7 +2661,7 @@
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>Şehitmustafa</v>
+        <v>Sucular</v>
       </c>
       <c r="B137" t="str">
         <v>RÜYA USLU</v>
@@ -1834,7 +2669,7 @@
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>Simithacılı</v>
+        <v>Şahin</v>
       </c>
       <c r="B138" t="str">
         <v>RÜYA USLU</v>
@@ -1842,7 +2677,7 @@
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>Sıraköy</v>
+        <v>Şehitisak</v>
       </c>
       <c r="B139" t="str">
         <v>RÜYA USLU</v>
@@ -1850,7 +2685,7 @@
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>Sofular</v>
+        <v>Şehitkerim</v>
       </c>
       <c r="B140" t="str">
         <v>RÜYA USLU</v>
@@ -1858,7 +2693,7 @@
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>Sucular</v>
+        <v>Şehitmustafa</v>
       </c>
       <c r="B141" t="str">
         <v>RÜYA USLU</v>
@@ -2082,7 +2917,7 @@
     </row>
     <row r="169">
       <c r="A169" t="str">
-        <v>Yüksek</v>
+        <v>Yunacık</v>
       </c>
       <c r="B169" t="str">
         <v>RÜYA USLU</v>
@@ -2090,7 +2925,7 @@
     </row>
     <row r="170">
       <c r="A170" t="str">
-        <v>Yunacık</v>
+        <v>Yunusoğlu</v>
       </c>
       <c r="B170" t="str">
         <v>RÜYA USLU</v>
@@ -2098,7 +2933,7 @@
     </row>
     <row r="171">
       <c r="A171" t="str">
-        <v>Yunusoğlu</v>
+        <v>Yüksek</v>
       </c>
       <c r="B171" t="str">
         <v>RÜYA USLU</v>
@@ -2135,7 +2970,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E44"/>
   <sheetViews>
@@ -2510,7 +3345,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -2707,157 +3542,6 @@
   </sheetData>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:E14"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Mahalle Adı</v>
-      </c>
-      <c r="B1" t="str">
-        <v>GÖREVLİ PERSONEL</v>
-      </c>
-      <c r="C1" t="str">
-        <v>MEGSİS ONAY TARİHİ</v>
-      </c>
-      <c r="D1" t="str">
-        <v>NETİGMA ONAY TARİHİ</v>
-      </c>
-      <c r="E1" t="str">
-        <v>MÜDÜR ONAY</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Bağçatağı</v>
-      </c>
-      <c r="B2" t="str">
-        <v>M. FURKAN KAPLAN</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Belçınar</v>
-      </c>
-      <c r="B3" t="str">
-        <v>M. FURKAN KAPLAN</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Çayırekinliği</v>
-      </c>
-      <c r="B4" t="str">
-        <v>M. FURKAN KAPLAN</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Cumayakası</v>
-      </c>
-      <c r="B5" t="str">
-        <v>M. FURKAN KAPLAN</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Darıpınarı</v>
-      </c>
-      <c r="B6" t="str">
-        <v>M. FURKAN KAPLAN</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Fakılar</v>
-      </c>
-      <c r="B7" t="str">
-        <v>M. FURKAN KAPLAN</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Giden</v>
-      </c>
-      <c r="B8" t="str">
-        <v>M. FURKAN KAPLAN</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Kale</v>
-      </c>
-      <c r="B9" t="str">
-        <v>RÜYA USLU</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>Kisecik</v>
-      </c>
-      <c r="B10" t="str">
-        <v>RÜYA USLU</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>Körmenlik</v>
-      </c>
-      <c r="B11" t="str">
-        <v>RÜYA USLU</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>Körüstan</v>
-      </c>
-      <c r="B12" t="str">
-        <v>RÜYA USLU</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>Namrun</v>
-      </c>
-      <c r="B13" t="str">
-        <v>RÜYA USLU</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>Sarıkavak</v>
-      </c>
-      <c r="B14" t="str">
-        <v>RÜYA USLU</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>Sarıkoyak</v>
-      </c>
-      <c r="B15" t="str">
-        <v>RÜYA USLU</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>Sebil</v>
-      </c>
-      <c r="B16" t="str">
-        <v>RÜYA USLU</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E16"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3217,7 +3901,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>Köprübaşı</v>
+        <v>Korucuk</v>
       </c>
       <c r="B42" t="str">
         <v>HÜSEYİN BÜYÜK</v>
@@ -3225,7 +3909,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>Korucuk</v>
+        <v>Köprübaşı</v>
       </c>
       <c r="B43" t="str">
         <v>HÜSEYİN BÜYÜK</v>
@@ -3257,7 +3941,7 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>Ören/batıkent</v>
+        <v>Ormancık</v>
       </c>
       <c r="B47" t="str">
         <v>HÜSEYİN BÜYÜK</v>
@@ -3265,7 +3949,7 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>Ören/kuzeyyurt</v>
+        <v>Ortaköy</v>
       </c>
       <c r="B48" t="str">
         <v>HÜSEYİN BÜYÜK</v>
@@ -3273,7 +3957,7 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>Ören/nasraddin</v>
+        <v>Ovabaşı</v>
       </c>
       <c r="B49" t="str">
         <v>HÜSEYİN BÜYÜK</v>
@@ -3281,7 +3965,7 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>Ören/ortaköy</v>
+        <v>Ören/batıkent</v>
       </c>
       <c r="B50" t="str">
         <v>HÜSEYİN BÜYÜK</v>
@@ -3289,7 +3973,7 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>Ormancık</v>
+        <v>Ören/kuzeyyurt</v>
       </c>
       <c r="B51" t="str">
         <v>HÜSEYİN BÜYÜK</v>
@@ -3297,7 +3981,7 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>Ortaköy</v>
+        <v>Ören/nasraddin</v>
       </c>
       <c r="B52" t="str">
         <v>HÜSEYİN BÜYÜK</v>
@@ -3305,7 +3989,7 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>Ovabaşı</v>
+        <v>Ören/ortaköy</v>
       </c>
       <c r="B53" t="str">
         <v>HÜSEYİN BÜYÜK</v>
@@ -3822,6 +4506,157 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Mahalle Adı</v>
+      </c>
+      <c r="B1" t="str">
+        <v>GÖREVLİ PERSONEL</v>
+      </c>
+      <c r="C1" t="str">
+        <v>MEGSİS ONAY TARİHİ</v>
+      </c>
+      <c r="D1" t="str">
+        <v>NETİGMA ONAY TARİHİ</v>
+      </c>
+      <c r="E1" t="str">
+        <v>MÜDÜR ONAY</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Bağçatağı</v>
+      </c>
+      <c r="B2" t="str">
+        <v>M. FURKAN KAPLAN</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Belçınar</v>
+      </c>
+      <c r="B3" t="str">
+        <v>M. FURKAN KAPLAN</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Cumayakası</v>
+      </c>
+      <c r="B4" t="str">
+        <v>M. FURKAN KAPLAN</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Çayırekinliği</v>
+      </c>
+      <c r="B5" t="str">
+        <v>M. FURKAN KAPLAN</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Darıpınarı</v>
+      </c>
+      <c r="B6" t="str">
+        <v>M. FURKAN KAPLAN</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Fakılar</v>
+      </c>
+      <c r="B7" t="str">
+        <v>M. FURKAN KAPLAN</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Giden</v>
+      </c>
+      <c r="B8" t="str">
+        <v>M. FURKAN KAPLAN</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Kale</v>
+      </c>
+      <c r="B9" t="str">
+        <v>RÜYA USLU</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Kisecik</v>
+      </c>
+      <c r="B10" t="str">
+        <v>RÜYA USLU</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Körmenlik</v>
+      </c>
+      <c r="B11" t="str">
+        <v>RÜYA USLU</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Körüstan</v>
+      </c>
+      <c r="B12" t="str">
+        <v>RÜYA USLU</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Namrun</v>
+      </c>
+      <c r="B13" t="str">
+        <v>RÜYA USLU</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Sarıkavak</v>
+      </c>
+      <c r="B14" t="str">
+        <v>RÜYA USLU</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Sarıkoyak</v>
+      </c>
+      <c r="B15" t="str">
+        <v>RÜYA USLU</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Sebil</v>
+      </c>
+      <c r="B16" t="str">
+        <v>RÜYA USLU</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:E16"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4178,7 +5013,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>Kösbucağı</v>
+        <v>Koyuncu</v>
       </c>
       <c r="B42" t="str">
         <v>SERDAR ARSLAN</v>
@@ -4186,7 +5021,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>Köserelli</v>
+        <v>Kösbucağı</v>
       </c>
       <c r="B43" t="str">
         <v>SERDAR ARSLAN</v>
@@ -4194,7 +5029,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>Koyuncu</v>
+        <v>Köserelli</v>
       </c>
       <c r="B44" t="str">
         <v>SERDAR ARSLAN</v>
@@ -4298,7 +5133,7 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>Şahna</v>
+        <v>Sarıkaya</v>
       </c>
       <c r="B57" t="str">
         <v>SERDAR ARSLAN</v>
@@ -4306,7 +5141,7 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>Sarıkaya</v>
+        <v>Sarıyer</v>
       </c>
       <c r="B58" t="str">
         <v>SERDAR ARSLAN</v>
@@ -4314,7 +5149,7 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>Sarıyer</v>
+        <v>Sıraç</v>
       </c>
       <c r="B59" t="str">
         <v>SERDAR ARSLAN</v>
@@ -4330,7 +5165,7 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>Sıraç</v>
+        <v>Sorgun</v>
       </c>
       <c r="B61" t="str">
         <v>SERDAR ARSLAN</v>
@@ -4338,7 +5173,7 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>Sorgun</v>
+        <v>Şahna</v>
       </c>
       <c r="B62" t="str">
         <v>SERDAR ARSLAN</v>
@@ -4370,7 +5205,7 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>Tömük</v>
+        <v>Toros</v>
       </c>
       <c r="B66" t="str">
         <v>SERDAR ARSLAN</v>
@@ -4378,7 +5213,7 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>Toros</v>
+        <v>Tömük</v>
       </c>
       <c r="B67" t="str">
         <v>SERDAR ARSLAN</v>
@@ -4459,7 +5294,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E55"/>
   <sheetViews>
@@ -4557,7 +5392,7 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Çavuşlar</v>
+        <v>Cumhuriyet</v>
       </c>
       <c r="B11" t="str">
         <v>BURAK AKBAŞ</v>
@@ -4565,7 +5400,7 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Çukurasma</v>
+        <v>Çavuşlar</v>
       </c>
       <c r="B12" t="str">
         <v>BURAK AKBAŞ</v>
@@ -4573,7 +5408,7 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Çukurkonak</v>
+        <v>Çukurasma</v>
       </c>
       <c r="B13" t="str">
         <v>BURAK AKBAŞ</v>
@@ -4581,7 +5416,7 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Cumhuriyet</v>
+        <v>Çukurkonak</v>
       </c>
       <c r="B14" t="str">
         <v>BURAK AKBAŞ</v>
@@ -4677,7 +5512,7 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>İshaklar</v>
+        <v>Işıklı</v>
       </c>
       <c r="B26" t="str">
         <v>BURAK AKBAŞ</v>
@@ -4685,7 +5520,7 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Işıklı</v>
+        <v>İshaklar</v>
       </c>
       <c r="B27" t="str">
         <v>BURAK AKBAŞ</v>
@@ -4821,7 +5656,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>Şeyhömer</v>
+        <v>Sipahili</v>
       </c>
       <c r="B44" t="str">
         <v>BURAK AKBAŞ</v>
@@ -4829,7 +5664,7 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>Sipahili</v>
+        <v>Sütlüce(kasaba)</v>
       </c>
       <c r="B45" t="str">
         <v>BURAK AKBAŞ</v>
@@ -4837,7 +5672,7 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>Sütlüce(kasaba)</v>
+        <v>Şeyhömer</v>
       </c>
       <c r="B46" t="str">
         <v>BURAK AKBAŞ</v>
@@ -4869,7 +5704,7 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>Üçoluk</v>
+        <v>Ulupınar</v>
       </c>
       <c r="B50" t="str">
         <v>BURAK AKBAŞ</v>
@@ -4877,7 +5712,7 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>Ulupınar</v>
+        <v>Üçoluk</v>
       </c>
       <c r="B51" t="str">
         <v>BURAK AKBAŞ</v>
@@ -4922,7 +5757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E24"/>
   <sheetViews>
@@ -5137,7 +5972,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E101"/>
   <sheetViews>
@@ -5235,7 +6070,7 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Çağlayangedik</v>
+        <v>Civciv</v>
       </c>
       <c r="B11" t="str">
         <v>ÖMER ÇEVİK</v>
@@ -5243,7 +6078,7 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Çakallı</v>
+        <v>Çağlayangedik</v>
       </c>
       <c r="B12" t="str">
         <v>ÖMER ÇEVİK</v>
@@ -5251,7 +6086,7 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Çaltılı</v>
+        <v>Çakallı</v>
       </c>
       <c r="B13" t="str">
         <v>ÖMER ÇEVİK</v>
@@ -5259,7 +6094,7 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Çamlıca</v>
+        <v>Çaltılı</v>
       </c>
       <c r="B14" t="str">
         <v>ÖMER ÇEVİK</v>
@@ -5267,7 +6102,7 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Çampınar</v>
+        <v>Çamlıca</v>
       </c>
       <c r="B15" t="str">
         <v>ÖMER ÇEVİK</v>
@@ -5275,7 +6110,7 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Çatakbağ</v>
+        <v>Çampınar</v>
       </c>
       <c r="B16" t="str">
         <v>ÖMER ÇEVİK</v>
@@ -5283,7 +6118,7 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Çatalharman</v>
+        <v>Çatakbağ</v>
       </c>
       <c r="B17" t="str">
         <v>ÖMER ÇEVİK</v>
@@ -5291,7 +6126,7 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Civciv</v>
+        <v>Çatalharman</v>
       </c>
       <c r="B18" t="str">
         <v>ÖMER ÇEVİK</v>
@@ -5307,7 +6142,7 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>Çömelek</v>
+        <v>Çortak</v>
       </c>
       <c r="B20" t="str">
         <v>ÖMER ÇEVİK</v>
@@ -5315,7 +6150,7 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>Çortak</v>
+        <v>Çömelek</v>
       </c>
       <c r="B21" t="str">
         <v>ÖMER ÇEVİK</v>
@@ -5563,7 +6398,7 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>İbrahimli</v>
+        <v>Işıklar</v>
       </c>
       <c r="B52" t="str">
         <v>ÖMER ÇEVİK</v>
@@ -5571,7 +6406,7 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>İlice</v>
+        <v>İbrahimli</v>
       </c>
       <c r="B53" t="str">
         <v>ÖMER ÇEVİK</v>
@@ -5579,7 +6414,7 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>Işıklar</v>
+        <v>İlice</v>
       </c>
       <c r="B54" t="str">
         <v>ÖMER ÇEVİK</v>
@@ -5723,7 +6558,7 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>Kültür</v>
+        <v>Kumaçukuru</v>
       </c>
       <c r="B72" t="str">
         <v>HİLMİ MÜFTÜOĞLU</v>
@@ -5731,7 +6566,7 @@
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>Kumaçukuru</v>
+        <v>Kurtuluş</v>
       </c>
       <c r="B73" t="str">
         <v>HİLMİ MÜFTÜOĞLU</v>
@@ -5739,7 +6574,7 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>Kürkçü</v>
+        <v>Kültür</v>
       </c>
       <c r="B74" t="str">
         <v>HİLMİ MÜFTÜOĞLU</v>
@@ -5747,7 +6582,7 @@
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>Kurtuluş</v>
+        <v>Kürkçü</v>
       </c>
       <c r="B75" t="str">
         <v>HİLMİ MÜFTÜOĞLU</v>
@@ -5966,836 +6801,4 @@
     <ignoredError numberStoredAsText="1" sqref="A1:E101"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E94"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Mahalle Adı</v>
-      </c>
-      <c r="B1" t="str">
-        <v>GÖREVLİ PERSONEL</v>
-      </c>
-      <c r="C1" t="str">
-        <v>MEGSİS ONAY TARİHİ</v>
-      </c>
-      <c r="D1" t="str">
-        <v>NETİGMA ONAY TARİHİ</v>
-      </c>
-      <c r="E1" t="str">
-        <v>MÜDÜR ONAY</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Akdere</v>
-      </c>
-      <c r="B2" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Akdere/atatürk</v>
-      </c>
-      <c r="B3" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Akdere/cumhuriyet</v>
-      </c>
-      <c r="B4" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Altınkum</v>
-      </c>
-      <c r="B5" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Arkarası</v>
-      </c>
-      <c r="B6" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Atik</v>
-      </c>
-      <c r="B7" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Ayaş türkmenli</v>
-      </c>
-      <c r="B8" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Bahçe</v>
-      </c>
-      <c r="B9" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>Bahçederesi</v>
-      </c>
-      <c r="B10" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>Balandız</v>
-      </c>
-      <c r="B11" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>Bayındır</v>
-      </c>
-      <c r="B12" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>Bolacalıkoyuncu</v>
-      </c>
-      <c r="B13" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>Boynuinceli</v>
-      </c>
-      <c r="B14" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>Bucaklı</v>
-      </c>
-      <c r="B15" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>Bükdeğirmeni</v>
-      </c>
-      <c r="B16" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>Burunucu</v>
-      </c>
-      <c r="B17" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>Çadırlı</v>
-      </c>
-      <c r="B18" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>Çaltıbozkır</v>
-      </c>
-      <c r="B19" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v>Cambazlı</v>
-      </c>
-      <c r="B20" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="str">
-        <v>Camikebir</v>
-      </c>
-      <c r="B21" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="str">
-        <v>Çamlıbel</v>
-      </c>
-      <c r="B22" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="str">
-        <v>Çatak</v>
-      </c>
-      <c r="B23" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="str">
-        <v>Çeltikçi</v>
-      </c>
-      <c r="B24" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="str">
-        <v>Cılbayır</v>
-      </c>
-      <c r="B25" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="str">
-        <v>Demircili</v>
-      </c>
-      <c r="B26" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-      <c r="C26" t="str">
-        <v>2025-09-30</v>
-      </c>
-      <c r="D26" t="str">
-        <v>2025-10-02</v>
-      </c>
-      <c r="E26" t="str">
-        <v>2025-10-03</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="str">
-        <v>Ekşiler</v>
-      </c>
-      <c r="B27" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="str">
-        <v>Esenbel</v>
-      </c>
-      <c r="B28" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="str">
-        <v>Evkafçiftliği</v>
-      </c>
-      <c r="B29" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="str">
-        <v>Gazi</v>
-      </c>
-      <c r="B30" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="str">
-        <v>Gedikpınarı</v>
-      </c>
-      <c r="B31" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="str">
-        <v>Gökbelen</v>
-      </c>
-      <c r="B32" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="str">
-        <v>Gülümpaşalı</v>
-      </c>
-      <c r="B33" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="str">
-        <v>Gümüşlü</v>
-      </c>
-      <c r="B34" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="str">
-        <v>Gündüzler</v>
-      </c>
-      <c r="B35" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="str">
-        <v>Hacıishaklı</v>
-      </c>
-      <c r="B36" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="str">
-        <v>Hasanaliler</v>
-      </c>
-      <c r="B37" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="str">
-        <v>Hırmanlı</v>
-      </c>
-      <c r="B38" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="str">
-        <v>Hüseyinler</v>
-      </c>
-      <c r="B39" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="str">
-        <v>İmambekirli</v>
-      </c>
-      <c r="B40" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="str">
-        <v>İmamlı</v>
-      </c>
-      <c r="B41" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-      <c r="C41" t="str">
-        <v>2025-10-01</v>
-      </c>
-      <c r="D41" t="str">
-        <v>2025-10-02</v>
-      </c>
-      <c r="E41" t="str">
-        <v>2025-10-03</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="str">
-        <v>İmamuşağı</v>
-      </c>
-      <c r="B42" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="str">
-        <v>Işıklı</v>
-      </c>
-      <c r="B43" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="str">
-        <v>Kabasakallı</v>
-      </c>
-      <c r="B44" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="str">
-        <v>Kapızlı</v>
-      </c>
-      <c r="B45" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="str">
-        <v>Karadedeli</v>
-      </c>
-      <c r="B46" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="str">
-        <v>Karahacılı</v>
-      </c>
-      <c r="B47" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="str">
-        <v>Karakaya</v>
-      </c>
-      <c r="B48" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="str">
-        <v>Kargıcak</v>
-      </c>
-      <c r="B49" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="str">
-        <v>Kavak</v>
-      </c>
-      <c r="B50" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="str">
-        <v>Keben</v>
-      </c>
-      <c r="B51" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="str">
-        <v>Kepez</v>
-      </c>
-      <c r="B52" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="str">
-        <v>Keşlitürkmenli</v>
-      </c>
-      <c r="B53" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-      <c r="C53" t="str">
-        <v>2025-10-01</v>
-      </c>
-      <c r="D53" t="str">
-        <v>2025-10-02</v>
-      </c>
-      <c r="E53" t="str">
-        <v>2025-10-02</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="str">
-        <v>Kıca</v>
-      </c>
-      <c r="B54" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="str">
-        <v>Kızılgeçit</v>
-      </c>
-      <c r="B55" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="str">
-        <v>Kızılisalı</v>
-      </c>
-      <c r="B56" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-      <c r="C56" t="str">
-        <v>2025-10-02</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="str">
-        <v>Kocaoluk</v>
-      </c>
-      <c r="B57" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="str">
-        <v>Kocapınar</v>
-      </c>
-      <c r="B58" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="str">
-        <v>Kurtuluş</v>
-      </c>
-      <c r="B59" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="str">
-        <v>Mara</v>
-      </c>
-      <c r="B60" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="str">
-        <v>Mukaddem</v>
-      </c>
-      <c r="B61" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="str">
-        <v>Mukaddem (a1)</v>
-      </c>
-      <c r="B62" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="str">
-        <v>Mukaddem(afet)</v>
-      </c>
-      <c r="B63" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="str">
-        <v>Nasrullah</v>
-      </c>
-      <c r="B64" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="str">
-        <v>Nuru</v>
-      </c>
-      <c r="B65" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="str">
-        <v>Olukbaşı</v>
-      </c>
-      <c r="B66" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="str">
-        <v>Ören</v>
-      </c>
-      <c r="B67" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="str">
-        <v>Ortaören</v>
-      </c>
-      <c r="B68" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="str">
-        <v>Ovacık</v>
-      </c>
-      <c r="B69" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-      <c r="C69" t="str">
-        <v>2025-10-02</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="str">
-        <v>Özboyuninceli</v>
-      </c>
-      <c r="B70" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="str">
-        <v>Öztürkmenli</v>
-      </c>
-      <c r="B71" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-      <c r="C71" t="str">
-        <v>2025-10-01</v>
-      </c>
-      <c r="D71" t="str">
-        <v>2025-10-02</v>
-      </c>
-      <c r="E71" t="str">
-        <v>2025-10-02</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="str">
-        <v>Pazarkaşı</v>
-      </c>
-      <c r="B72" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="str">
-        <v>Pelitpınarı</v>
-      </c>
-      <c r="B73" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="str">
-        <v>Sabak</v>
-      </c>
-      <c r="B74" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="str">
-        <v>Şahmurlu</v>
-      </c>
-      <c r="B75" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="str">
-        <v>Saray</v>
-      </c>
-      <c r="B76" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="str">
-        <v>Sarıaydın</v>
-      </c>
-      <c r="B77" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="str">
-        <v>Sarıcalar</v>
-      </c>
-      <c r="B78" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="str">
-        <v>Say</v>
-      </c>
-      <c r="B79" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="str">
-        <v>Sayağzı</v>
-      </c>
-      <c r="B80" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="str">
-        <v>Senir</v>
-      </c>
-      <c r="B81" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="str">
-        <v>Seydili</v>
-      </c>
-      <c r="B82" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="str">
-        <v>Seyranlık</v>
-      </c>
-      <c r="B83" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="str">
-        <v>Sökün</v>
-      </c>
-      <c r="B84" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="str">
-        <v>Sömek</v>
-      </c>
-      <c r="B85" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="str">
-        <v>Susanoğlu</v>
-      </c>
-      <c r="B86" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="str">
-        <v>Taşucu</v>
-      </c>
-      <c r="B87" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="str">
-        <v>Tosmurlu</v>
-      </c>
-      <c r="B88" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="str">
-        <v>Türkmenuşağı</v>
-      </c>
-      <c r="B89" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-      <c r="C89" t="str">
-        <v>2025-10-01</v>
-      </c>
-      <c r="D89" t="str">
-        <v>2025-10-02</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="str">
-        <v>Ulugöz</v>
-      </c>
-      <c r="B90" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="str">
-        <v>Uzuncaburç</v>
-      </c>
-      <c r="B91" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="str">
-        <v>Yeğenli</v>
-      </c>
-      <c r="B92" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="str">
-        <v>Yenibahçe</v>
-      </c>
-      <c r="B93" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-      <c r="C93" t="str">
-        <v>2025-10-01</v>
-      </c>
-      <c r="D93" t="str">
-        <v>2025-10-02</v>
-      </c>
-      <c r="E93" t="str">
-        <v>2025-10-02</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="str">
-        <v>Yenisu</v>
-      </c>
-      <c r="B94" t="str">
-        <v>BURAK AKBAŞ</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E94"/>
-  </ignoredErrors>
-</worksheet>
 </file>
</xml_diff>